<commit_message>
mlwn ahu y3m kamal
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20115\Dropbox\My PC (LAPTOP-ILAL93NC)\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD35C4C-1D4A-4B33-8669-8D209E6029E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2612D4-17E7-4943-A91B-4CD560A919A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,10 +84,38 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -121,6 +149,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +436,7 @@
   <dimension ref="A1:R159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +575,7 @@
       <c r="B6">
         <v>1095</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>3704.8</v>
       </c>
       <c r="D6">
@@ -586,10 +618,10 @@
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>1111</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>1954.3</v>
       </c>
       <c r="D8">
@@ -598,7 +630,7 @@
       <c r="E8">
         <v>17545.7</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>75.538239000000004</v>
       </c>
       <c r="R8">
@@ -609,7 +641,7 @@
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>135</v>
       </c>
       <c r="C9">
@@ -621,7 +653,7 @@
       <c r="E9">
         <v>16844.5</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>20.279098999999999</v>
       </c>
       <c r="R9">

</xml_diff>